<commit_message>
UI integrations with excel download
</commit_message>
<xml_diff>
--- a/uploads/addLabels.xlsx
+++ b/uploads/addLabels.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Language_id</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Label_value</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -448,25 +451,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>